<commit_message>
Update new function and request
Use quantile to filter outlier
Add the intercept in LR equation
Able to change the column in easy way
</commit_message>
<xml_diff>
--- a/Testdata.xlsx
+++ b/Testdata.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -435,31 +435,31 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <v>3</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
       <c r="H2">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -467,63 +467,63 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1">
-        <v>101</v>
+        <v>175</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H3">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I3">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>7</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
       <c r="H4">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="I4">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -531,7 +531,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -543,27 +543,27 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H5">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I5">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1">
-        <v>284</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -575,19 +575,19 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H6">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="I6">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1">
-        <v>218</v>
+        <v>260</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -604,22 +604,22 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>4</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
       <c r="H7">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -627,16 +627,16 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1">
-        <v>32</v>
+        <v>206</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -645,77 +645,77 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1">
-        <v>60</v>
+        <v>272</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
+        <v>11</v>
+      </c>
+      <c r="H9">
+        <v>55</v>
+      </c>
+      <c r="I9">
         <v>4</v>
       </c>
-      <c r="H9">
-        <v>40</v>
-      </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1">
-        <v>254</v>
+        <v>87</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H10">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="I10">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1">
-        <v>313</v>
+        <v>0</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -732,54 +732,54 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
+        <v>1.5</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
         <v>8</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>7</v>
-      </c>
       <c r="H11">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I11">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
         <v>2</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>11</v>
-      </c>
       <c r="H12">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="I12">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -787,51 +787,51 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1">
-        <v>336</v>
+        <v>298</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H13">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="I13">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="J13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1">
-        <v>86</v>
+        <v>161</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -840,10 +840,10 @@
         <v>5</v>
       </c>
       <c r="H14">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I14">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -863,19 +863,19 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H15">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I15">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -883,7 +883,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1">
-        <v>333</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -892,22 +892,22 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H16">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="I16">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1">
-        <v>249</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -927,19 +927,19 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H17">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="I17">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -947,7 +947,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -959,19 +959,19 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H18">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="I18">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -988,120 +988,24 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H19">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="I19">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="1">
-        <v>92</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>11</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>13</v>
-      </c>
-      <c r="H20">
-        <v>59</v>
-      </c>
-      <c r="I20">
-        <v>8</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="1">
-        <v>138</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>3</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>3</v>
-      </c>
-      <c r="H21">
-        <v>29</v>
-      </c>
-      <c r="I21">
-        <v>3</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="1">
-        <v>31</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>3</v>
-      </c>
-      <c r="H22">
-        <v>34</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
         <v>0</v>
       </c>
     </row>

</xml_diff>